<commit_message>
fix: Update CORS configuration to allow multiple frontend URLs
</commit_message>
<xml_diff>
--- a/data/RECONOCIMIENTO.xlsx
+++ b/data/RECONOCIMIENTO.xlsx
@@ -1294,7 +1294,7 @@
     <t>TEXTO_SUGERENCIA</t>
   </si>
   <si>
-    <t>ACTIVO</t>
+    <t>CUANDO_APLICA</t>
   </si>
   <si>
     <t>FLAG_ACTIVO</t>
@@ -1563,7 +1563,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1591,7 +1590,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1601,6 +1600,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6985,6 +6987,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="38.22"/>
+    <col customWidth="1" min="4" max="4" width="67.44"/>
+    <col customWidth="1" min="5" max="5" width="49.11"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -6999,7 +7006,7 @@
       <c r="D1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>424</v>
       </c>
       <c r="F1" s="1" t="s">

</xml_diff>